<commit_message>
Adding a document about ISA.
</commit_message>
<xml_diff>
--- a/examples/extract/MS_colon_measurements_truncated.xlsx
+++ b/examples/extract/MS_colon_measurements_truncated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\examples\extract\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01237F8E-2B1E-416D-ADC5-1AFBF4BC7A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4362FF2-1725-4C01-94E4-F1E7C2730C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1350" windowWidth="21720" windowHeight="12975" activeTab="1" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
+    <workbookView xWindow="4560" yWindow="1485" windowWidth="21720" windowHeight="12975" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
   </bookViews>
   <sheets>
     <sheet name="#automate" sheetId="5" r:id="rId1"/>
@@ -4564,9 +4564,6 @@
     <t xml:space="preserve">Dionex IonPac AS11-HC-4um 2 mm i.d. x 250 mm </t>
   </si>
   <si>
-    <t>IC-FTMS_measurement</t>
-  </si>
-  <si>
     <t>#end</t>
   </si>
   <si>
@@ -4637,6 +4634,9 @@
   </si>
   <si>
     <t>#.machine_type</t>
+  </si>
+  <si>
+    <t>labeled_IC-FTMS_measurement</t>
   </si>
 </sst>
 </file>
@@ -5010,8 +5010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F8C4CA-E64B-495F-8E50-4DEE3E196AA7}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5035,7 +5035,7 @@
         <v>1486</v>
       </c>
       <c r="G2" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="H2" t="s">
         <v>1487</v>
@@ -5065,7 +5065,7 @@
         <v>1495</v>
       </c>
       <c r="R2" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5073,7 +5073,7 @@
         <v>1496</v>
       </c>
       <c r="F3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="G3" t="s">
         <v>1497</v>
@@ -5106,12 +5106,12 @@
         <v>1504</v>
       </c>
       <c r="R3" t="s">
-        <v>1506</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -5119,26 +5119,26 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D8" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D9" t="s">
         <v>1509</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1510</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D10" t="s">
         <v>1511</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1512</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -5146,7 +5146,7 @@
         <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -5154,7 +5154,7 @@
         <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -5162,15 +5162,15 @@
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D14" t="s">
         <v>1515</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1516</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -5178,7 +5178,7 @@
         <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -5186,7 +5186,7 @@
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -5194,7 +5194,7 @@
         <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -5202,20 +5202,20 @@
         <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D19" t="s">
         <v>1521</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1522</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
   </sheetData>
@@ -5227,8 +5227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44723B69-977D-4B94-80FA-9A2DD691D416}">
   <dimension ref="A1:S151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13751,7 +13751,7 @@
         <v>197</v>
       </c>
       <c r="E1" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -13888,10 +13888,10 @@
         <v>197</v>
       </c>
       <c r="E18" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="F18" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -14028,7 +14028,7 @@
         <v>197</v>
       </c>
       <c r="E36" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="F36" t="s">
         <v>232</v>
@@ -15275,7 +15275,7 @@
         <v>197</v>
       </c>
       <c r="E108" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>